<commit_message>
Correction to Form Name
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_N_devolucao/ILRG_ORAM_N_devolucao-media/ILRG_ORAM_N_devolucao.xlsx
+++ b/ILRG_ORAM_N_devolucao/ILRG_ORAM_N_devolucao-media/ILRG_ORAM_N_devolucao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\oram\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_N_devolucao\ILRG_ORAM_N_devolucao-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66122D0-FCA9-4787-A9C3-E240E94F62DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1901DC0A-28E9-4A00-A0FE-E915DAC87B97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3598,9 +3598,6 @@
     <t>Escreve o seu apelido se não apareceu na lista</t>
   </si>
   <si>
-    <t>"Formulário N - Cartograma"</t>
-  </si>
-  <si>
     <t>Ng1</t>
   </si>
   <si>
@@ -3794,15 +3791,25 @@
   </si>
   <si>
     <t>${birthdate_y_n_2} = 'no'</t>
+  </si>
+  <si>
+    <t>"Formulário N - Devolução"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4006,413 +4013,414 @@
   </borders>
   <cellStyleXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="240" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="240" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="240"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="240" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="240" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="240" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="240"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="241">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4994,11 +5002,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G60" sqref="G60"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,8 +5106,8 @@
       <c r="B5" s="66" t="s">
         <v>1087</v>
       </c>
-      <c r="M5" s="49" t="s">
-        <v>1187</v>
+      <c r="M5" s="79" t="s">
+        <v>1252</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5107,7 +5115,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C6" s="2"/>
       <c r="L6" s="49" t="s">
@@ -5175,7 +5183,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1181</v>
@@ -5283,7 +5291,7 @@
     </row>
     <row r="19" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>1104</v>
@@ -5309,10 +5317,10 @@
         <v>1092</v>
       </c>
       <c r="C20" s="69" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D20" s="69" t="s">
         <v>1191</v>
-      </c>
-      <c r="D20" s="69" t="s">
-        <v>1192</v>
       </c>
       <c r="J20" s="69" t="s">
         <v>22</v>
@@ -5326,7 +5334,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C21" s="45" t="s">
         <v>1090</v>
@@ -5343,13 +5351,13 @@
         <v>34</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -5357,7 +5365,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>68</v>
@@ -5371,7 +5379,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C24" s="49" t="s">
         <v>88</v>
@@ -5385,7 +5393,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C25" s="49" t="s">
         <v>89</v>
@@ -5399,7 +5407,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C26" s="49" t="s">
         <v>90</v>
@@ -5419,13 +5427,13 @@
     </row>
     <row r="28" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B28" s="75" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C28" s="49" t="s">
         <v>1203</v>
-      </c>
-      <c r="B28" s="75" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>1204</v>
       </c>
       <c r="J28" s="49" t="s">
         <v>22</v>
@@ -5439,10 +5447,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C29" s="72" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="L29" s="26" t="s">
         <v>33</v>
@@ -5453,13 +5461,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="65" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C30" s="49" t="s">
         <v>1205</v>
       </c>
-      <c r="C30" s="49" t="s">
-        <v>1206</v>
-      </c>
       <c r="G30" s="76" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="L30" s="49" t="s">
         <v>45</v>
@@ -5470,13 +5478,13 @@
         <v>73</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C31" s="49" t="s">
         <v>91</v>
       </c>
       <c r="G31" s="76" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="L31" s="49" t="s">
         <v>70</v>
@@ -5493,7 +5501,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="67" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>74</v>
@@ -5507,7 +5515,7 @@
         <v>40</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C34" s="49" t="s">
         <v>69</v>
@@ -5524,16 +5532,16 @@
         <v>31</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C35" s="49" t="s">
         <v>44</v>
       </c>
       <c r="H35" s="49" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I35" s="49" t="s">
         <v>1210</v>
-      </c>
-      <c r="I35" s="49" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5541,16 +5549,16 @@
         <v>31</v>
       </c>
       <c r="B36" s="65" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C36" s="49" t="s">
         <v>1212</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="H36" s="49" t="s">
         <v>1213</v>
       </c>
-      <c r="H36" s="49" t="s">
-        <v>1214</v>
-      </c>
       <c r="I36" s="49" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5558,10 +5566,10 @@
         <v>17</v>
       </c>
       <c r="B37" s="65" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C37" s="49" t="s">
         <v>1215</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>1216</v>
       </c>
       <c r="L37" s="49" t="s">
         <v>45</v>
@@ -5572,10 +5580,10 @@
         <v>17</v>
       </c>
       <c r="B38" s="65" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C38" s="49" t="s">
         <v>1217</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>1218</v>
       </c>
       <c r="L38" s="49" t="s">
         <v>45</v>
@@ -5583,13 +5591,13 @@
     </row>
     <row r="39" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B39" s="65" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C39" s="49" t="s">
         <v>1219</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5603,7 +5611,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C41" s="49" t="s">
         <v>71</v>
@@ -5620,7 +5628,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J42" s="49" t="s">
         <v>22</v>
@@ -5634,10 +5642,10 @@
         <v>32</v>
       </c>
       <c r="B43" s="65" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C43" s="49" t="s">
         <v>1223</v>
-      </c>
-      <c r="C43" s="49" t="s">
-        <v>1224</v>
       </c>
       <c r="J43" s="49" t="s">
         <v>22</v>
@@ -5648,10 +5656,10 @@
         <v>32</v>
       </c>
       <c r="B44" s="65" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C44" s="49" t="s">
         <v>1225</v>
-      </c>
-      <c r="C44" s="49" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -5659,13 +5667,13 @@
         <v>31</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C45" s="31" t="s">
         <v>92</v>
       </c>
       <c r="H45" s="49" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5673,16 +5681,16 @@
         <v>31</v>
       </c>
       <c r="B46" s="65" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C46" s="49" t="s">
         <v>1227</v>
       </c>
-      <c r="C46" s="49" t="s">
+      <c r="H46" s="49" t="s">
         <v>1228</v>
       </c>
-      <c r="H46" s="49" t="s">
+      <c r="L46" s="49" t="s">
         <v>1229</v>
-      </c>
-      <c r="L46" s="49" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -5707,7 +5715,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="71" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C49" s="31" t="s">
         <v>86</v>
@@ -5719,13 +5727,13 @@
         <v>34</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C50" s="31" t="s">
         <v>87</v>
       </c>
       <c r="E50" s="72" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -5733,7 +5741,7 @@
         <v>23</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C51" s="26" t="s">
         <v>68</v>
@@ -5747,7 +5755,7 @@
         <v>31</v>
       </c>
       <c r="B52" s="71" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C52" s="72" t="s">
         <v>88</v>
@@ -5761,7 +5769,7 @@
         <v>31</v>
       </c>
       <c r="B53" s="71" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C53" s="72" t="s">
         <v>89</v>
@@ -5775,7 +5783,7 @@
         <v>72</v>
       </c>
       <c r="B54" s="71" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C54" s="72" t="s">
         <v>90</v>
@@ -5795,13 +5803,13 @@
     </row>
     <row r="56" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="72" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B56" s="77" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C56" s="72" t="s">
         <v>1203</v>
-      </c>
-      <c r="B56" s="77" t="s">
-        <v>1250</v>
-      </c>
-      <c r="C56" s="72" t="s">
-        <v>1204</v>
       </c>
       <c r="J56" s="72" t="s">
         <v>22</v>
@@ -5815,10 +5823,10 @@
         <v>23</v>
       </c>
       <c r="B57" s="41" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C57" s="72" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="L57" s="26" t="s">
         <v>33</v>
@@ -5829,13 +5837,13 @@
         <v>17</v>
       </c>
       <c r="B58" s="71" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C58" s="72" t="s">
         <v>1205</v>
       </c>
-      <c r="C58" s="72" t="s">
-        <v>1206</v>
-      </c>
       <c r="G58" s="78" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="L58" s="72" t="s">
         <v>45</v>
@@ -5846,13 +5854,13 @@
         <v>73</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C59" s="72" t="s">
         <v>91</v>
       </c>
       <c r="G59" s="78" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="L59" s="72" t="s">
         <v>70</v>
@@ -5869,7 +5877,7 @@
         <v>23</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>74</v>
@@ -5883,7 +5891,7 @@
         <v>40</v>
       </c>
       <c r="B62" s="71" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C62" s="72" t="s">
         <v>69</v>
@@ -5900,16 +5908,16 @@
         <v>31</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>44</v>
       </c>
       <c r="H63" s="72" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I63" s="72" t="s">
         <v>1210</v>
-      </c>
-      <c r="I63" s="72" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -5917,16 +5925,16 @@
         <v>31</v>
       </c>
       <c r="B64" s="71" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C64" s="72" t="s">
         <v>1212</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="H64" s="72" t="s">
         <v>1213</v>
       </c>
-      <c r="H64" s="72" t="s">
-        <v>1214</v>
-      </c>
       <c r="I64" s="72" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -5934,10 +5942,10 @@
         <v>17</v>
       </c>
       <c r="B65" s="71" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C65" s="72" t="s">
         <v>1215</v>
-      </c>
-      <c r="C65" s="72" t="s">
-        <v>1216</v>
       </c>
       <c r="L65" s="72" t="s">
         <v>45</v>
@@ -5948,10 +5956,10 @@
         <v>17</v>
       </c>
       <c r="B66" s="71" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C66" s="72" t="s">
         <v>1217</v>
-      </c>
-      <c r="C66" s="72" t="s">
-        <v>1218</v>
       </c>
       <c r="L66" s="72" t="s">
         <v>45</v>
@@ -5959,13 +5967,13 @@
     </row>
     <row r="67" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="72" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B67" s="71" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C67" s="72" t="s">
         <v>1219</v>
-      </c>
-      <c r="C67" s="72" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="68" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -5979,7 +5987,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="71" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C69" s="72" t="s">
         <v>71</v>
@@ -5996,7 +6004,7 @@
         <v>39</v>
       </c>
       <c r="C70" s="72" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J70" s="72" t="s">
         <v>22</v>
@@ -6010,10 +6018,10 @@
         <v>32</v>
       </c>
       <c r="B71" s="71" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C71" s="72" t="s">
         <v>1223</v>
-      </c>
-      <c r="C71" s="72" t="s">
-        <v>1224</v>
       </c>
       <c r="J71" s="72" t="s">
         <v>22</v>
@@ -6024,10 +6032,10 @@
         <v>32</v>
       </c>
       <c r="B72" s="71" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C72" s="72" t="s">
         <v>1225</v>
-      </c>
-      <c r="C72" s="72" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="73" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -6035,13 +6043,13 @@
         <v>31</v>
       </c>
       <c r="B73" s="71" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C73" s="31" t="s">
         <v>92</v>
       </c>
       <c r="H73" s="72" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -6049,16 +6057,16 @@
         <v>31</v>
       </c>
       <c r="B74" s="71" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C74" s="72" t="s">
         <v>1227</v>
       </c>
-      <c r="C74" s="72" t="s">
+      <c r="H74" s="72" t="s">
         <v>1228</v>
       </c>
-      <c r="H74" s="72" t="s">
+      <c r="L74" s="72" t="s">
         <v>1229</v>
-      </c>
-      <c r="L74" s="72" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
@@ -6083,10 +6091,10 @@
         <v>46</v>
       </c>
       <c r="B77" s="65" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C77" s="49" t="s">
         <v>1235</v>
-      </c>
-      <c r="C77" s="49" t="s">
-        <v>1236</v>
       </c>
       <c r="H77" s="49" t="s">
         <v>77</v>
@@ -6100,13 +6108,13 @@
         <v>34</v>
       </c>
       <c r="B78" s="67" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C78" s="49" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E78" s="49" t="s">
         <v>1237</v>
-      </c>
-      <c r="C78" s="49" t="s">
-        <v>1241</v>
-      </c>
-      <c r="E78" s="49" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6114,7 +6122,7 @@
         <v>67</v>
       </c>
       <c r="B79" s="65" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C79" s="49" t="s">
         <v>1180</v>
@@ -6131,7 +6139,7 @@
         <v>23</v>
       </c>
       <c r="B80" s="67" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>74</v>
@@ -6145,7 +6153,7 @@
         <v>40</v>
       </c>
       <c r="B81" s="65" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C81" s="49" t="s">
         <v>69</v>
@@ -6162,16 +6170,16 @@
         <v>31</v>
       </c>
       <c r="B82" s="65" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C82" s="49" t="s">
         <v>44</v>
       </c>
       <c r="H82" s="49" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I82" s="49" t="s">
         <v>1210</v>
-      </c>
-      <c r="I82" s="49" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6179,16 +6187,16 @@
         <v>31</v>
       </c>
       <c r="B83" s="65" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C83" s="49" t="s">
         <v>1212</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="H83" s="49" t="s">
         <v>1213</v>
       </c>
-      <c r="H83" s="49" t="s">
-        <v>1214</v>
-      </c>
       <c r="I83" s="49" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="84" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6196,10 +6204,10 @@
         <v>17</v>
       </c>
       <c r="B84" s="65" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C84" s="49" t="s">
         <v>1215</v>
-      </c>
-      <c r="C84" s="49" t="s">
-        <v>1216</v>
       </c>
       <c r="L84" s="49" t="s">
         <v>45</v>
@@ -6210,10 +6218,10 @@
         <v>17</v>
       </c>
       <c r="B85" s="65" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C85" s="49" t="s">
         <v>1217</v>
-      </c>
-      <c r="C85" s="49" t="s">
-        <v>1218</v>
       </c>
       <c r="L85" s="49" t="s">
         <v>45</v>
@@ -6221,13 +6229,13 @@
     </row>
     <row r="86" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="49" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B86" s="65" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C86" s="49" t="s">
         <v>1219</v>
-      </c>
-      <c r="C86" s="49" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="87" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6241,10 +6249,10 @@
         <v>32</v>
       </c>
       <c r="B88" s="65" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C88" s="49" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="J88" s="49" t="s">
         <v>22</v>
@@ -6258,7 +6266,7 @@
         <v>39</v>
       </c>
       <c r="C89" s="49" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J89" s="49" t="s">
         <v>22</v>
@@ -6272,10 +6280,10 @@
         <v>32</v>
       </c>
       <c r="B90" s="65" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C90" s="49" t="s">
         <v>1223</v>
-      </c>
-      <c r="C90" s="49" t="s">
-        <v>1224</v>
       </c>
       <c r="J90" s="49" t="s">
         <v>22</v>
@@ -6286,10 +6294,10 @@
         <v>32</v>
       </c>
       <c r="B91" s="65" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C91" s="49" t="s">
         <v>1225</v>
-      </c>
-      <c r="C91" s="49" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6297,16 +6305,16 @@
         <v>31</v>
       </c>
       <c r="B92" s="65" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C92" s="49" t="s">
         <v>1227</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="H92" s="49" t="s">
         <v>1228</v>
       </c>
-      <c r="H92" s="49" t="s">
+      <c r="L92" s="49" t="s">
         <v>1229</v>
-      </c>
-      <c r="L92" s="49" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -32348,8 +32356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32383,7 +32391,7 @@
         <v>1103</v>
       </c>
       <c r="C2" s="48">
-        <v>201904191</v>
+        <v>201904192</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>1095</v>

</xml_diff>